<commit_message>
80 - add option to switch between millisecond and seconds timer
</commit_message>
<xml_diff>
--- a/Tchoukball_Scoreboard_MJ/Tchoukball_Scoreboard_MJ/Resources/Template.xlsx
+++ b/Tchoukball_Scoreboard_MJ/Tchoukball_Scoreboard_MJ/Resources/Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repository\Tchoukball_Scoreboard_MJ\Tchoukball_Scoreboard_MJ\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repository\Tchoukball_Scoreboard_MJ\Tchoukball_Scoreboard_MJ\bin\Release\net8.0-windows\publish\win-x86\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC57F81-0F6D-4D12-B2F3-EF55A524DA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8F08DA-ED1A-48B2-9031-4F46D9E5C6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="624" windowWidth="22740" windowHeight="11508" xr2:uid="{22C2B78F-1732-4FAB-98EF-04FFC232478E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{22C2B78F-1732-4FAB-98EF-04FFC232478E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Home</t>
   </si>
@@ -48,15 +48,9 @@
     <t>A01</t>
   </si>
   <si>
-    <t>Open Men</t>
-  </si>
-  <si>
     <t>A02</t>
   </si>
   <si>
-    <t>U12</t>
-  </si>
-  <si>
     <t>CategoryColor</t>
   </si>
   <si>
@@ -66,85 +60,52 @@
     <t>12:00</t>
   </si>
   <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>01:00</t>
-  </si>
-  <si>
-    <t>Johor</t>
-  </si>
-  <si>
-    <t>Penang</t>
-  </si>
-  <si>
-    <t>Sarawak</t>
-  </si>
-  <si>
-    <t>Negeri Sembilan</t>
-  </si>
-  <si>
     <t>A03</t>
   </si>
   <si>
-    <t>10:01</t>
-  </si>
-  <si>
-    <t>01:01</t>
-  </si>
-  <si>
-    <t>U13</t>
-  </si>
-  <si>
     <t>A04</t>
   </si>
   <si>
-    <t>10:02</t>
-  </si>
-  <si>
-    <t>01:02</t>
-  </si>
-  <si>
-    <t>U14</t>
-  </si>
-  <si>
     <t>A05</t>
   </si>
   <si>
-    <t>10:03</t>
-  </si>
-  <si>
-    <t>01:03</t>
-  </si>
-  <si>
-    <t>U15</t>
-  </si>
-  <si>
     <t>A06</t>
   </si>
   <si>
-    <t>10:04</t>
-  </si>
-  <si>
-    <t>01:04</t>
-  </si>
-  <si>
-    <t>U16</t>
-  </si>
-  <si>
     <t>A07</t>
   </si>
   <si>
-    <t>10:05</t>
-  </si>
-  <si>
-    <t>01:05</t>
-  </si>
-  <si>
-    <t>U17</t>
-  </si>
-  <si>
-    <t>Selangor</t>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>U18 BOY</t>
+  </si>
+  <si>
+    <t>OPEN FEMALE</t>
+  </si>
+  <si>
+    <t>OPEN MALE</t>
+  </si>
+  <si>
+    <t>U18 GIRL</t>
+  </si>
+  <si>
+    <t>SELANGOR</t>
+  </si>
+  <si>
+    <t>JOHOR</t>
+  </si>
+  <si>
+    <t>PENANG</t>
+  </si>
+  <si>
+    <t>JOHOR 1</t>
+  </si>
+  <si>
+    <t>JOHOR 2</t>
+  </si>
+  <si>
+    <t>SARAWAK</t>
   </si>
 </sst>
 </file>
@@ -172,7 +133,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,31 +154,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF9900"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -234,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -242,9 +185,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,6 +193,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9900"/>
       <color rgb="FF969696"/>
       <color rgb="FF00FF99"/>
       <color rgb="FFCC6600"/>
@@ -566,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8315DDF-53C4-45C0-93F1-223F720C7719}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -605,147 +546,168 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="6"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>